<commit_message>
Added configuration images and updated documentation for v1.1.0 of the BF-88E.
</commit_message>
<xml_diff>
--- a/Documents/Radio Configuration Table BF-88E.xlsx
+++ b/Documents/Radio Configuration Table BF-88E.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelnetherway/GitWorkspace/BF-88E/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257B472C-2863-C44C-9CCA-25A29F5D8BA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8319346A-CD7D-3A46-8DFA-3EC27F50E08B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="24000" xr2:uid="{2F353EC1-3109-4D44-9297-7AF6286BFB6D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{2F353EC1-3109-4D44-9297-7AF6286BFB6D}"/>
   </bookViews>
   <sheets>
     <sheet name="v1.0.0" sheetId="1" r:id="rId1"/>
+    <sheet name="v1.0.1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="21">
   <si>
     <t>Frequency</t>
   </si>
@@ -140,7 +141,67 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="40">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -215,27 +276,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9342197A-6855-3B4C-A36B-604B959961DA}" name="Table1" displayName="Table1" ref="B2:S18" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9342197A-6855-3B4C-A36B-604B959961DA}" name="Table1" displayName="Table1" ref="B2:S18" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="B2:S18" xr:uid="{C17D325A-F6CF-6E45-9E03-FE14ECED045B}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{0F0DC48D-C7E9-2A46-9DC7-3682F15B042D}" name="Location" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{7603A102-6E5C-B04B-9B6F-F26375C8A809}" name="Name" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{D51AFB5A-8923-D343-A4F7-DDFA3918C662}" name="Frequency" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{D1223C4B-F031-E24C-9688-0321238B20B5}" name="Duplex" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{2E00CBBA-E069-034F-9DC4-8BF666A00DF6}" name="Offset" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{A6FDE082-7974-BA41-BFB8-5A9A12C6D07E}" name="Tone" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{FFE6335B-DC58-F94B-AB2C-8E23EAB1DBAC}" name="rToneFreq" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{90515244-BB70-0A42-9A2F-C54C8FC54C1A}" name="cToneFreq" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{0F4818F0-2E06-E346-97C5-C49340C88242}" name="DtcsCode" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{44EDBCB0-85A9-9948-8B6D-B9E561A84C27}" name="DtcsPolarity" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{CA847C26-C577-DB42-83D4-EFD10E64EBEA}" name="Mode" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{5A376B5B-76D9-F64A-9ACF-EB6D64657AE3}" name="TStep" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{81B663FC-DA31-F04F-BAA9-4D3C64225DEE}" name="Skip" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{72F0A697-99B8-5745-88BE-BDE0C988CF0F}" name="Comment" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{DA27DEA7-3387-934B-83C4-0B303EF79DD1}" name="URCALL" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{A24B1DFA-03D0-534B-BA02-4BB0F5916144}" name="RPT1CALL" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{94278AE7-9F61-F443-8905-2766BA862444}" name="RPT2CALL" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{3CB3454E-0AFE-2145-8612-3D407DE21899}" name="DVCODE" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0F0DC48D-C7E9-2A46-9DC7-3682F15B042D}" name="Location" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{7603A102-6E5C-B04B-9B6F-F26375C8A809}" name="Name" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{D51AFB5A-8923-D343-A4F7-DDFA3918C662}" name="Frequency" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{D1223C4B-F031-E24C-9688-0321238B20B5}" name="Duplex" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{2E00CBBA-E069-034F-9DC4-8BF666A00DF6}" name="Offset" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{A6FDE082-7974-BA41-BFB8-5A9A12C6D07E}" name="Tone" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{FFE6335B-DC58-F94B-AB2C-8E23EAB1DBAC}" name="rToneFreq" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{90515244-BB70-0A42-9A2F-C54C8FC54C1A}" name="cToneFreq" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{0F4818F0-2E06-E346-97C5-C49340C88242}" name="DtcsCode" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{44EDBCB0-85A9-9948-8B6D-B9E561A84C27}" name="DtcsPolarity" dataDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{CA847C26-C577-DB42-83D4-EFD10E64EBEA}" name="Mode" dataDxfId="27"/>
+    <tableColumn id="12" xr3:uid="{5A376B5B-76D9-F64A-9ACF-EB6D64657AE3}" name="TStep" dataDxfId="26"/>
+    <tableColumn id="13" xr3:uid="{81B663FC-DA31-F04F-BAA9-4D3C64225DEE}" name="Skip" dataDxfId="25"/>
+    <tableColumn id="14" xr3:uid="{72F0A697-99B8-5745-88BE-BDE0C988CF0F}" name="Comment" dataDxfId="24"/>
+    <tableColumn id="15" xr3:uid="{DA27DEA7-3387-934B-83C4-0B303EF79DD1}" name="URCALL" dataDxfId="23"/>
+    <tableColumn id="16" xr3:uid="{A24B1DFA-03D0-534B-BA02-4BB0F5916144}" name="RPT1CALL" dataDxfId="22"/>
+    <tableColumn id="17" xr3:uid="{94278AE7-9F61-F443-8905-2766BA862444}" name="RPT2CALL" dataDxfId="21"/>
+    <tableColumn id="18" xr3:uid="{3CB3454E-0AFE-2145-8612-3D407DE21899}" name="DVCODE" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2481E489-3102-3947-A669-57AAFA2DD54F}" name="Table13" displayName="Table13" ref="B2:S10" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="B2:S10" xr:uid="{C2DFA995-6FC1-374D-9FA4-09348FD8C908}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{9B8E4947-1FD0-8249-BF34-C4DED9E9C018}" name="Location" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{B33960D4-21B8-1B42-BC31-26D1EC11DBA4}" name="Name" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{6172BC22-5BE4-9E4F-8EA7-D3B91B603A07}" name="Frequency" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{BD6A69D3-DAB8-524D-882D-7A57AAE99736}" name="Duplex" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{C5ED89FB-F129-DB4F-B97A-A535066601B4}" name="Offset" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{2DD65DD2-864B-3943-A028-A4900BCB2549}" name="Tone" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{5E172B53-0EFB-A94B-A467-59D13497F926}" name="rToneFreq" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{C1683AB0-C49B-3C49-BFD8-6BE3D2A3CBA0}" name="cToneFreq" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{1983AF6E-8821-F94B-9E11-F557F9F4F595}" name="DtcsCode" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{DE7285EC-474F-584F-A1EB-C59BB29715BD}" name="DtcsPolarity" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{77B5C970-99F9-714B-80F7-A7F175E25E9B}" name="Mode" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{B68C56AE-3554-1843-973A-6A7DB84B94EB}" name="TStep" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{6DA77B3B-838E-6843-B907-3C7097338FDB}" name="Skip" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{AE6E3013-056C-5D46-BD15-2062D731ED1E}" name="Comment" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{E86C12E3-95BC-7F40-A368-B48C1016F2A7}" name="URCALL" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{27E83967-F4DF-514C-9CD5-F1DA39BCB0B0}" name="RPT1CALL" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{63006631-904B-4842-995E-EEDEB467FE6F}" name="RPT2CALL" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{CCF2756A-52CB-E14E-8BCB-AAF6FFE69B22}" name="DVCODE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -540,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462E0174-0307-0C48-97DD-F4613CE40FD8}">
   <dimension ref="B2:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1266,4 +1354,575 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78237EA-12AD-6342-A45C-0E0DD6E51397}">
+  <dimension ref="B2:S18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1">
+        <v>446.00625000000002</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I3" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J3" s="1">
+        <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
+        <v>446.01875000000001</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J4" s="1">
+        <v>23</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="1">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>446.03125</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>23</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
+        <v>446.04374999999999</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>23</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="1">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>446.05624999999998</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I7" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>23</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="1">
+        <v>5</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1">
+        <v>446.06875000000002</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>23</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="1">
+        <v>5</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
+        <v>446.08125000000001</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I9" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J9" s="1">
+        <v>23</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1">
+        <v>446.09375</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I10" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J10" s="1">
+        <v>23</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Amended version numbers to v1.1.0.
</commit_message>
<xml_diff>
--- a/Documents/Radio Configuration Table BF-88E.xlsx
+++ b/Documents/Radio Configuration Table BF-88E.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelnetherway/GitWorkspace/BF-88E/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8319346A-CD7D-3A46-8DFA-3EC27F50E08B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6C6677-E72D-2249-BDBF-7D4815251298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{2F353EC1-3109-4D44-9297-7AF6286BFB6D}"/>
   </bookViews>
   <sheets>
     <sheet name="v1.0.0" sheetId="1" r:id="rId1"/>
-    <sheet name="v1.0.1" sheetId="2" r:id="rId2"/>
+    <sheet name="v1.1.0" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>

<commit_message>
Added configuration image and updated documentation for v1.1.1 of the BF-88E. Updated Radio Configuration Table to have a TX power column.
</commit_message>
<xml_diff>
--- a/Documents/Radio Configuration Table BF-88E.xlsx
+++ b/Documents/Radio Configuration Table BF-88E.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelnetherway/GitWorkspace/BF-88E/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6C6677-E72D-2249-BDBF-7D4815251298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334D9B13-453E-6648-8056-3915211FCCEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{2F353EC1-3109-4D44-9297-7AF6286BFB6D}"/>
   </bookViews>
   <sheets>
     <sheet name="v1.0.0" sheetId="1" r:id="rId1"/>
     <sheet name="v1.1.0" sheetId="2" r:id="rId2"/>
+    <sheet name="v1.1.1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="24">
   <si>
     <t>Frequency</t>
   </si>
@@ -98,6 +99,15 @@
   <si>
     <t>S</t>
   </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
 </sst>
 </file>
 
@@ -141,7 +151,76 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="63">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -276,54 +355,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9342197A-6855-3B4C-A36B-604B959961DA}" name="Table1" displayName="Table1" ref="B2:S18" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
-  <autoFilter ref="B2:S18" xr:uid="{C17D325A-F6CF-6E45-9E03-FE14ECED045B}"/>
-  <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{0F0DC48D-C7E9-2A46-9DC7-3682F15B042D}" name="Location" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{7603A102-6E5C-B04B-9B6F-F26375C8A809}" name="Name" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{D51AFB5A-8923-D343-A4F7-DDFA3918C662}" name="Frequency" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{D1223C4B-F031-E24C-9688-0321238B20B5}" name="Duplex" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{2E00CBBA-E069-034F-9DC4-8BF666A00DF6}" name="Offset" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{A6FDE082-7974-BA41-BFB8-5A9A12C6D07E}" name="Tone" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{FFE6335B-DC58-F94B-AB2C-8E23EAB1DBAC}" name="rToneFreq" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{90515244-BB70-0A42-9A2F-C54C8FC54C1A}" name="cToneFreq" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{0F4818F0-2E06-E346-97C5-C49340C88242}" name="DtcsCode" dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{44EDBCB0-85A9-9948-8B6D-B9E561A84C27}" name="DtcsPolarity" dataDxfId="28"/>
-    <tableColumn id="11" xr3:uid="{CA847C26-C577-DB42-83D4-EFD10E64EBEA}" name="Mode" dataDxfId="27"/>
-    <tableColumn id="12" xr3:uid="{5A376B5B-76D9-F64A-9ACF-EB6D64657AE3}" name="TStep" dataDxfId="26"/>
-    <tableColumn id="13" xr3:uid="{81B663FC-DA31-F04F-BAA9-4D3C64225DEE}" name="Skip" dataDxfId="25"/>
-    <tableColumn id="14" xr3:uid="{72F0A697-99B8-5745-88BE-BDE0C988CF0F}" name="Comment" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{DA27DEA7-3387-934B-83C4-0B303EF79DD1}" name="URCALL" dataDxfId="23"/>
-    <tableColumn id="16" xr3:uid="{A24B1DFA-03D0-534B-BA02-4BB0F5916144}" name="RPT1CALL" dataDxfId="22"/>
-    <tableColumn id="17" xr3:uid="{94278AE7-9F61-F443-8905-2766BA862444}" name="RPT2CALL" dataDxfId="21"/>
-    <tableColumn id="18" xr3:uid="{3CB3454E-0AFE-2145-8612-3D407DE21899}" name="DVCODE" dataDxfId="20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9342197A-6855-3B4C-A36B-604B959961DA}" name="Table1" displayName="Table1" ref="B2:T18" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+  <autoFilter ref="B2:T18" xr:uid="{C17D325A-F6CF-6E45-9E03-FE14ECED045B}"/>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{0F0DC48D-C7E9-2A46-9DC7-3682F15B042D}" name="Location" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{7603A102-6E5C-B04B-9B6F-F26375C8A809}" name="Name" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{D51AFB5A-8923-D343-A4F7-DDFA3918C662}" name="Frequency" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{D1223C4B-F031-E24C-9688-0321238B20B5}" name="Duplex" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{2E00CBBA-E069-034F-9DC4-8BF666A00DF6}" name="Offset" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{A6FDE082-7974-BA41-BFB8-5A9A12C6D07E}" name="Tone" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{FFE6335B-DC58-F94B-AB2C-8E23EAB1DBAC}" name="rToneFreq" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{90515244-BB70-0A42-9A2F-C54C8FC54C1A}" name="cToneFreq" dataDxfId="53"/>
+    <tableColumn id="9" xr3:uid="{0F4818F0-2E06-E346-97C5-C49340C88242}" name="DtcsCode" dataDxfId="52"/>
+    <tableColumn id="10" xr3:uid="{44EDBCB0-85A9-9948-8B6D-B9E561A84C27}" name="DtcsPolarity" dataDxfId="51"/>
+    <tableColumn id="11" xr3:uid="{CA847C26-C577-DB42-83D4-EFD10E64EBEA}" name="Mode" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{5A376B5B-76D9-F64A-9ACF-EB6D64657AE3}" name="TStep" dataDxfId="49"/>
+    <tableColumn id="19" xr3:uid="{B104A57F-9E4E-8040-B7A2-6C57396CD674}" name="Power" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{81B663FC-DA31-F04F-BAA9-4D3C64225DEE}" name="Skip" dataDxfId="48"/>
+    <tableColumn id="14" xr3:uid="{72F0A697-99B8-5745-88BE-BDE0C988CF0F}" name="Comment" dataDxfId="47"/>
+    <tableColumn id="15" xr3:uid="{DA27DEA7-3387-934B-83C4-0B303EF79DD1}" name="URCALL" dataDxfId="46"/>
+    <tableColumn id="16" xr3:uid="{A24B1DFA-03D0-534B-BA02-4BB0F5916144}" name="RPT1CALL" dataDxfId="45"/>
+    <tableColumn id="17" xr3:uid="{94278AE7-9F61-F443-8905-2766BA862444}" name="RPT2CALL" dataDxfId="44"/>
+    <tableColumn id="18" xr3:uid="{3CB3454E-0AFE-2145-8612-3D407DE21899}" name="DVCODE" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2481E489-3102-3947-A669-57AAFA2DD54F}" name="Table13" displayName="Table13" ref="B2:S10" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="B2:S10" xr:uid="{C2DFA995-6FC1-374D-9FA4-09348FD8C908}"/>
-  <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{9B8E4947-1FD0-8249-BF34-C4DED9E9C018}" name="Location" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{B33960D4-21B8-1B42-BC31-26D1EC11DBA4}" name="Name" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{6172BC22-5BE4-9E4F-8EA7-D3B91B603A07}" name="Frequency" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{BD6A69D3-DAB8-524D-882D-7A57AAE99736}" name="Duplex" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{C5ED89FB-F129-DB4F-B97A-A535066601B4}" name="Offset" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{2DD65DD2-864B-3943-A028-A4900BCB2549}" name="Tone" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{5E172B53-0EFB-A94B-A467-59D13497F926}" name="rToneFreq" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{C1683AB0-C49B-3C49-BFD8-6BE3D2A3CBA0}" name="cToneFreq" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{1983AF6E-8821-F94B-9E11-F557F9F4F595}" name="DtcsCode" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{DE7285EC-474F-584F-A1EB-C59BB29715BD}" name="DtcsPolarity" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{77B5C970-99F9-714B-80F7-A7F175E25E9B}" name="Mode" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{B68C56AE-3554-1843-973A-6A7DB84B94EB}" name="TStep" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{6DA77B3B-838E-6843-B907-3C7097338FDB}" name="Skip" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{AE6E3013-056C-5D46-BD15-2062D731ED1E}" name="Comment" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{E86C12E3-95BC-7F40-A368-B48C1016F2A7}" name="URCALL" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{27E83967-F4DF-514C-9CD5-F1DA39BCB0B0}" name="RPT1CALL" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{63006631-904B-4842-995E-EEDEB467FE6F}" name="RPT2CALL" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{CCF2756A-52CB-E14E-8BCB-AAF6FFE69B22}" name="DVCODE" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2481E489-3102-3947-A669-57AAFA2DD54F}" name="Table13" displayName="Table13" ref="B2:T10" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+  <autoFilter ref="B2:T10" xr:uid="{C2DFA995-6FC1-374D-9FA4-09348FD8C908}"/>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{9B8E4947-1FD0-8249-BF34-C4DED9E9C018}" name="Location" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{B33960D4-21B8-1B42-BC31-26D1EC11DBA4}" name="Name" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{6172BC22-5BE4-9E4F-8EA7-D3B91B603A07}" name="Frequency" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{BD6A69D3-DAB8-524D-882D-7A57AAE99736}" name="Duplex" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{C5ED89FB-F129-DB4F-B97A-A535066601B4}" name="Offset" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{2DD65DD2-864B-3943-A028-A4900BCB2549}" name="Tone" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{5E172B53-0EFB-A94B-A467-59D13497F926}" name="rToneFreq" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{C1683AB0-C49B-3C49-BFD8-6BE3D2A3CBA0}" name="cToneFreq" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{1983AF6E-8821-F94B-9E11-F557F9F4F595}" name="DtcsCode" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{DE7285EC-474F-584F-A1EB-C59BB29715BD}" name="DtcsPolarity" dataDxfId="31"/>
+    <tableColumn id="11" xr3:uid="{77B5C970-99F9-714B-80F7-A7F175E25E9B}" name="Mode" dataDxfId="30"/>
+    <tableColumn id="12" xr3:uid="{B68C56AE-3554-1843-973A-6A7DB84B94EB}" name="TStep" dataDxfId="29"/>
+    <tableColumn id="19" xr3:uid="{861BD319-7F6F-194B-9399-DAF8EB02270F}" name="Power" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{6DA77B3B-838E-6843-B907-3C7097338FDB}" name="Skip" dataDxfId="28"/>
+    <tableColumn id="14" xr3:uid="{AE6E3013-056C-5D46-BD15-2062D731ED1E}" name="Comment" dataDxfId="27"/>
+    <tableColumn id="15" xr3:uid="{E86C12E3-95BC-7F40-A368-B48C1016F2A7}" name="URCALL" dataDxfId="26"/>
+    <tableColumn id="16" xr3:uid="{27E83967-F4DF-514C-9CD5-F1DA39BCB0B0}" name="RPT1CALL" dataDxfId="25"/>
+    <tableColumn id="17" xr3:uid="{63006631-904B-4842-995E-EEDEB467FE6F}" name="RPT2CALL" dataDxfId="24"/>
+    <tableColumn id="18" xr3:uid="{CCF2756A-52CB-E14E-8BCB-AAF6FFE69B22}" name="DVCODE" dataDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4AB36631-73A5-CA46-AEFF-E1D32FAA9DF9}" name="Table134" displayName="Table134" ref="B2:T10" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="B2:T10" xr:uid="{3E90F1EF-0744-5A4C-BF32-D918E645FD95}"/>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{06FB1734-1FDE-4044-AC1F-101AB2366FA8}" name="Location" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{521385BF-09AB-8D42-82D2-09B9ADA1FF4F}" name="Name" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{5EC58422-3F68-144B-84F5-3D582DE70636}" name="Frequency" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{1987C51F-4C18-E34A-8B5D-5AD15CF9CE5D}" name="Duplex" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{A9A06FBD-ECB5-FD4F-9CB9-A4E129F31FF0}" name="Offset" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{AD12F86E-8992-1B47-AAAA-3C67E1F809CF}" name="Tone" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{E9ECC8D1-3753-5F42-89FB-7100C07940A0}" name="rToneFreq" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{9309F301-7954-9442-AB74-D161E21EAB6A}" name="cToneFreq" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{B759F7DD-DDFE-034D-AA38-3C9E20D98398}" name="DtcsCode" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{8D11EC36-A357-9E49-921F-1D45C9DDF952}" name="DtcsPolarity" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{AA722DBE-2C47-5944-923E-8F9423CC37F3}" name="Mode" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{51139972-128B-504F-AC20-7A1881E86B24}" name="TStep" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{C788489E-9760-844B-8E61-32485DE82F43}" name="Power" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{49C75EE1-1A9B-0D4A-B46F-A8E5BB0D973F}" name="Skip" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{C398310F-CA52-A840-9B3E-9A5588CD54E7}" name="Comment" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{7C03AED5-6167-B84D-8C3C-9D67AC6B7B2A}" name="URCALL" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{A278CCEA-D6A9-8D4E-9B36-0E5CEEFD7B8A}" name="RPT1CALL" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{342BC72A-583E-A547-A9AD-B1F62CB8B5F7}" name="RPT2CALL" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{BBF9D541-23CB-0A4E-99F8-195555CC176A}" name="DVCODE" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -626,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462E0174-0307-0C48-97DD-F4613CE40FD8}">
-  <dimension ref="B2:S18"/>
+  <dimension ref="B2:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:S18"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,14 +754,14 @@
     <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
@@ -690,25 +799,28 @@
         <v>12</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -740,15 +852,18 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -780,15 +895,18 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -820,15 +938,18 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -860,15 +981,18 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -900,15 +1024,18 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -940,15 +1067,18 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O8" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -980,15 +1110,18 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O9" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -1020,15 +1153,18 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O10" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -1060,15 +1196,18 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O11" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -1100,15 +1239,18 @@
         <v>5</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O12" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -1140,15 +1282,18 @@
         <v>5</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -1180,15 +1325,18 @@
         <v>5</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O14" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -1220,15 +1368,18 @@
         <v>5</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O15" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T15" s="1"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -1260,15 +1411,18 @@
         <v>5</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O16" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -1300,15 +1454,18 @@
         <v>5</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O17" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -1340,13 +1497,16 @@
         <v>5</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O18" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1358,10 +1518,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78237EA-12AD-6342-A45C-0E0DD6E51397}">
-  <dimension ref="B2:S18"/>
+  <dimension ref="B2:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1376,14 +1536,14 @@
     <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1421,25 +1581,28 @@
         <v>12</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1471,15 +1634,18 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -1511,15 +1677,18 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -1551,15 +1720,18 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -1591,15 +1763,18 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -1631,15 +1806,18 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -1671,15 +1849,18 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O8" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -1711,15 +1892,18 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O9" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -1751,15 +1935,18 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O10" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1779,7 +1966,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1799,7 +1986,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1819,7 +2006,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1839,7 +2026,7 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1859,7 +2046,7 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1925,4 +2112,443 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526AE6F0-8A6A-2E44-8918-A0EC5729C367}">
+  <dimension ref="B2:T10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1">
+        <v>446.00625000000002</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I3" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J3" s="1">
+        <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
+        <v>446.01875000000001</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J4" s="1">
+        <v>23</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="1">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>446.03125</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>23</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
+        <v>446.04374999999999</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>23</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="1">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>446.05624999999998</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I7" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>23</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="1">
+        <v>5</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1">
+        <v>446.06875000000002</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>23</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="1">
+        <v>5</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
+        <v>446.08125000000001</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I9" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J9" s="1">
+        <v>23</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1">
+        <v>446.09375</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I10" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J10" s="1">
+        <v>23</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>